<commit_message>
update: update database core
</commit_message>
<xml_diff>
--- a/database_apartment.xlsx
+++ b/database_apartment.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\management_apartment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stone/apartment_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81ACFDF1-6323-4EF6-9F8F-AEBEEC6641C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F01E182-39DC-B149-B313-B4FE406D6250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8815590B-3217-411B-B580-FB522E055A2D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="60160" windowHeight="31720" xr2:uid="{8815590B-3217-411B-B580-FB522E055A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="user " sheetId="1" r:id="rId1"/>
     <sheet name="apartment" sheetId="2" r:id="rId2"/>
-    <sheet name="customers " sheetId="3" r:id="rId3"/>
-    <sheet name="bookings " sheetId="4" r:id="rId4"/>
-    <sheet name="product" sheetId="5" r:id="rId5"/>
-    <sheet name="supplie" sheetId="6" r:id="rId6"/>
-    <sheet name="importProduct" sheetId="7" r:id="rId7"/>
+    <sheet name="apartment_owner" sheetId="8" r:id="rId3"/>
+    <sheet name="owner_image" sheetId="9" r:id="rId4"/>
+    <sheet name="customers " sheetId="3" r:id="rId5"/>
+    <sheet name="bookings " sheetId="4" r:id="rId6"/>
+    <sheet name="product" sheetId="5" r:id="rId7"/>
+    <sheet name="suppliers" sheetId="6" r:id="rId8"/>
+    <sheet name="importProduct" sheetId="7" r:id="rId9"/>
+    <sheet name="contract extension" sheetId="10" r:id="rId10"/>
+    <sheet name="customers_image" sheetId="11" r:id="rId11"/>
+    <sheet name="apartment_image" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -97,12 +102,6 @@
     <t>số CCCD defauld null</t>
   </si>
   <si>
-    <t>1: 1 phòng ngủ
-2
-3
-4</t>
-  </si>
-  <si>
     <t>status (enum)</t>
   </si>
   <si>
@@ -122,9 +121,6 @@
   </si>
   <si>
     <t>date of birth default null</t>
-  </si>
-  <si>
-    <t>nguồn user.id</t>
   </si>
   <si>
     <t>check_in date (date) defauld null</t>
@@ -207,41 +203,216 @@
     <t>product.id</t>
   </si>
   <si>
-    <t>supplie.id</t>
-  </si>
-  <si>
     <t>1: available
 2: reserved
 3: checked_in
 4: not available</t>
   </si>
   <si>
-    <t>rent_start_time</t>
-  </si>
-  <si>
-    <t>rent_end_time</t>
-  </si>
-  <si>
-    <t>house_owner_name</t>
-  </si>
-  <si>
-    <t>house_owner_phone_number</t>
-  </si>
-  <si>
     <t>phone_number</t>
+  </si>
+  <si>
+    <t>rent_price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>apartment_owner.id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>full_name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>area (int)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>appliances_price (int)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rent_price (int)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rent_start_time (date)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rent_end_time (date)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>create_at</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>update_at</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id (CCCD)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>image_file_name</t>
+  </si>
+  <si>
+    <t>image_file_name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>user.id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>suppliers.id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>apartment.id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date_of_extension</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>customers.id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>1: 1 phòng ng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ủ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2: 2 phòng ng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ủ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3: 3 phòng ng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ủ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+4: 4 phòng ng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ủ</t>
+    </r>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -265,16 +436,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -290,7 +462,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -608,24 +780,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4D1616-59CB-4E61-B2BE-D36B83A21114}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="30.625" customWidth="1"/>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
-    <col min="3" max="4" width="15.75" customWidth="1"/>
-    <col min="5" max="5" width="16.125" customWidth="1"/>
-    <col min="6" max="6" width="16.375" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="8" width="23.5" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="20.75" customWidth="1"/>
-    <col min="11" max="11" width="18.25" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -660,7 +832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="76.5" customHeight="1">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -668,35 +840,151 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="I20" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE55C121-6946-134C-9B83-03F5D439B823}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P66" sqref="P66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F17BCE20-2EAF-F645-9829-39B16465BFD0}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48134150-8C7B-534A-AA1F-69B19CDAE85B}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C599B7C8-6D08-48A5-B297-1112D32294F4}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="17.75" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="28.375" customWidth="1"/>
-    <col min="6" max="8" width="30.25" customWidth="1"/>
-    <col min="9" max="10" width="15.5" customWidth="1"/>
-    <col min="11" max="11" width="11.375" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="3" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="10" width="30.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -707,105 +995,188 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:14" ht="97.5" customHeight="1">
       <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D6488F-EABE-BA49-9498-F6F0106BF4EF}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6542DB-C6F4-A943-8DBF-62C8CABFE4D7}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573F3E80-90CC-4FA4-91F8-86DF6CC245B7}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1669F9-F75C-4202-9266-6E383BFDD2BD}">
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -813,94 +1184,95 @@
       <selection activeCell="L18" sqref="L18:L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
-    <col min="2" max="2" width="23.125" customWidth="1"/>
-    <col min="3" max="3" width="24.625" customWidth="1"/>
-    <col min="4" max="4" width="18.75" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
-    <col min="6" max="8" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="11" width="17.25" customWidth="1"/>
-    <col min="12" max="12" width="11.875" customWidth="1"/>
-    <col min="13" max="13" width="11.75" customWidth="1"/>
+    <col min="10" max="11" width="17.1640625" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="76">
+      <c r="F10" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="57" x14ac:dyDescent="0.2">
-      <c r="F10" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="K10" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD957D2-40EC-458B-9250-D4B0FE90B342}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -908,119 +1280,123 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
     <col min="6" max="6" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE43E02-66A2-4D39-B566-F83AE9726105}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
-    <col min="3" max="3" width="15.75" customWidth="1"/>
-    <col min="5" max="5" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
-        <v>47</v>
-      </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032E9F35-51A8-4374-94C6-55805B4788B9}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
-    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6">
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="E3" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>